<commit_message>
chore: snapshot 2026-02-07 (exclude local env/backups)
</commit_message>
<xml_diff>
--- a/backend/templates/repair_task_library_import_template.xlsx
+++ b/backend/templates/repair_task_library_import_template.xlsx
@@ -447,42 +447,42 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>????</t>
+          <t>任务名称</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>????</t>
+          <t>任务类别</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>????</t>
+          <t>给分方式</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>????</t>
+          <t>单位积分</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>??</t>
+          <t>数量</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>????</t>
+          <t>积分规则</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>???????</t>
+          <t>数量是否可修改</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>???????</t>
+          <t>积分是否可修改</t>
         </is>
       </c>
     </row>
@@ -505,12 +505,20 @@
       <c r="D2" t="n">
         <v>10</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>备注说明</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>否</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>否</t>
         </is>
@@ -542,108 +550,108 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>??</t>
+          <t>表头</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>????</t>
+          <t>填写说明</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>????</t>
+          <t>任务名称</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>?????????????????</t>
+          <t>必填，任务名称，不能重复。</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>????</t>
+          <t>任务类别</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>?????????????/??</t>
+          <t>选填，自由文本，用于筛选区分。</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>????</t>
+          <t>给分方式</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>?????? ????? / ??? / ???</t>
+          <t>选填，填写 奖扣结合式 / 扣分项 / 奖分项。</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>????</t>
+          <t>单位积分</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>?????????/?/0????10?-5</t>
+          <t>必填，数字，可为正/负/0，示例 10 / -5。</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>??</t>
+          <t>数量</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>???????? 1-1000????1?2</t>
+          <t>选填，1-1000 的整数，默认 1。</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>????</t>
+          <t>积分规则</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>???????? 200 ??????????</t>
+          <t>选填，备注说明。</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>???????</t>
+          <t>数量是否可修改</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>????? ?/?</t>
+          <t>选填，填写 是/否，默认 否。</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>???????</t>
+          <t>积分是否可修改</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>????? ?/?</t>
+          <t>选填，填写 是/否，默认 否。</t>
         </is>
       </c>
     </row>

</xml_diff>